<commit_message>
Process charges for OUAA donors.  Generate final report spreadsheet.
</commit_message>
<xml_diff>
--- a/db/pledgesummary_1341776587.xlsx
+++ b/db/pledgesummary_1341776587.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-24580" yWindow="-280" windowWidth="20820" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="-21920" yWindow="-360" windowWidth="20820" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="pledgesummary_1341776587.csv" sheetId="1" r:id="rId1"/>
@@ -1276,8 +1276,16 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1305,10 +1313,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1642,7 +1653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G143"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1655,26 +1668,26 @@
     <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>